<commit_message>
cleaning up datasets and resulting code housekeeping
</commit_message>
<xml_diff>
--- a/1979_Bradfield_ORIGINAL.xlsx
+++ b/1979_Bradfield_ORIGINAL.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20373"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20387"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_F25DC773A252ABEACE02EC789B5E440E5BDE589C" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{A39E57A4-0606-47AE-B1EB-B9CFF9ECCB1F}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="11_F25DC773A252ABEACE02EC789B5E440E5BDE589C" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{4B78261C-0F25-4925-A516-7F335A2564F9}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -70,169 +70,169 @@
     <t>SPECIES/QUADRAT NUMBER</t>
   </si>
   <si>
-    <t>Agrostis alba</t>
+    <t>Agrostis_alba</t>
   </si>
   <si>
-    <t>Alisma plantago-aquatica</t>
+    <t>Alisma_plantago-aquatica</t>
   </si>
   <si>
-    <t>Alopecurus geniculatus</t>
+    <t>Alopecurus_geniculatus</t>
   </si>
   <si>
-    <t>Oenanthe sarmentosa</t>
+    <t>Oenanthe_sarmentosa</t>
   </si>
   <si>
-    <t>Aster eatonii</t>
+    <t>Aster_eatonii</t>
   </si>
   <si>
-    <t>Bidens cernua</t>
+    <t>Bidens_cernua</t>
   </si>
   <si>
-    <t>Caltha palustris</t>
+    <t>Caltha_palustris</t>
   </si>
   <si>
-    <t>Carex lyngbei</t>
+    <t>Carex_lyngbei</t>
   </si>
   <si>
-    <t>Cirsium arvense</t>
+    <t>Cirsium_arvense</t>
   </si>
   <si>
-    <t>Deschampsia caespitosa</t>
+    <t>Deschampsia_caespitosa</t>
   </si>
   <si>
-    <t>Dulichium arundinaceum</t>
+    <t>Dulichium_arundinaceum</t>
   </si>
   <si>
-    <t>Eleocharis palustris</t>
+    <t>Eleocharis_palustris</t>
   </si>
   <si>
-    <t>Equisetum variegatum</t>
+    <t>Equisetum_variegatum</t>
   </si>
   <si>
-    <t>Equisetum fluviatile</t>
+    <t>Equisetum_fluviatile</t>
   </si>
   <si>
-    <t>Equisetum palustre</t>
+    <t>Equisetum_palustre</t>
   </si>
   <si>
-    <t>Festuca arundinacea</t>
+    <t>Festuca_arundinacea</t>
   </si>
   <si>
-    <t>Festuca sp.</t>
+    <t>Galium_cymosum</t>
   </si>
   <si>
-    <t>Galium cymosum</t>
+    <t>Platanthera_dilatata</t>
   </si>
   <si>
-    <t>Platanthera dilatata</t>
+    <t>Hordeum_brachyantherum</t>
   </si>
   <si>
-    <t>Hordeum brachyantherum</t>
+    <t>Hypericum_formosum</t>
   </si>
   <si>
-    <t>Hypericum formosum</t>
+    <t>Impatiens_capensis</t>
   </si>
   <si>
-    <t>Impatiens capensis</t>
+    <t>Juncus_articulatus</t>
   </si>
   <si>
-    <t>Juncus articulatus</t>
+    <t>Juncus_effusus</t>
   </si>
   <si>
-    <t>Juncus effusus</t>
+    <t>Juncus_oxymeris</t>
   </si>
   <si>
-    <t>Juncus oxymeris</t>
+    <t>Lathyrus_palustris</t>
   </si>
   <si>
-    <t>Lathyrus palustris</t>
+    <t>Leersia_oryzoides</t>
   </si>
   <si>
-    <t>Leersia oryzoides</t>
+    <t>Lilaeopsis_occidentalis</t>
   </si>
   <si>
-    <t>Lilaeopsis occidentalis</t>
+    <t>Lilaea_scilloides</t>
   </si>
   <si>
-    <t>Lilaea scilloides</t>
+    <t>Lysimachia_thyrsiflora</t>
   </si>
   <si>
-    <t>Lysimachia thyrsiflora</t>
+    <t>Lythrum_salicaria</t>
   </si>
   <si>
-    <t>Lythrum salicaria</t>
+    <t>Mentha_arvensis</t>
   </si>
   <si>
-    <t>Mentha arvensis</t>
+    <t>Menyanthes_trifoliata</t>
   </si>
   <si>
-    <t>Menyanthes trifoliata</t>
+    <t>Mimulus_guttatus</t>
   </si>
   <si>
-    <t>Mimulus guttatus</t>
+    <t>Myosotis_scorpioides</t>
   </si>
   <si>
-    <t>Myosotis scorpioides</t>
+    <t>Phalaris_arundinacea</t>
   </si>
   <si>
-    <t>Phalaris arundinacea</t>
+    <t>Poa_palustris</t>
   </si>
   <si>
-    <t>Poa palustris</t>
+    <t>Poa_trivialis</t>
   </si>
   <si>
-    <t>Poa trivialis</t>
+    <t>Polygonum_hydropiper</t>
   </si>
   <si>
-    <t>Polygonum hydropiper</t>
+    <t>Potentilla_pacifica</t>
   </si>
   <si>
-    <t>Potentilla pacifica</t>
+    <t>Puccinella_pauciflora</t>
   </si>
   <si>
-    <t>Puccinella pauciflora</t>
+    <t>Mentha_citrata</t>
   </si>
   <si>
-    <t>Mentha citrata</t>
+    <t>Rumex_conglomeratus</t>
   </si>
   <si>
-    <t>Rumex conglomeratus</t>
+    <t>Rumex_occidentalis</t>
   </si>
   <si>
-    <t>Rumex occidentalis</t>
+    <t>Sagittaria_latifolia</t>
   </si>
   <si>
-    <t>Sagittaria latifolia</t>
+    <t>Salix_lasiandra</t>
   </si>
   <si>
-    <t>Salix lasiandra</t>
+    <t>Salix_sitchensis</t>
   </si>
   <si>
-    <t>Salix sitchensis</t>
+    <t>Scirpus_validus</t>
   </si>
   <si>
-    <t>Salix sp.</t>
+    <t>Sidalcea_hendersonii</t>
   </si>
   <si>
-    <t>Scirpus validus</t>
+    <t>Sium_suave</t>
   </si>
   <si>
-    <t>Sidalcea hendersonii</t>
+    <t>Sonchus_arvensis</t>
   </si>
   <si>
-    <t>Sium suave</t>
+    <t>Trifolium_wormskjoldii</t>
   </si>
   <si>
-    <t>Sonchus arvensis</t>
+    <t>Typha_latifolia</t>
   </si>
   <si>
-    <t>Trifolium wormskjoldii</t>
+    <t>Zannichellia_palustris</t>
   </si>
   <si>
-    <t>Typha latifolia</t>
+    <t>Festuca_sp</t>
   </si>
   <si>
-    <t>Zannichellia palustris</t>
+    <t>Salix_sp</t>
   </si>
 </sst>
 </file>
@@ -663,11 +663,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DE58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="A59" sqref="A59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="35.36328125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:109" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
@@ -6720,7 +6723,7 @@
     </row>
     <row r="20" spans="1:109" x14ac:dyDescent="0.35">
       <c r="A20" s="14" t="s">
-        <v>32</v>
+        <v>69</v>
       </c>
       <c r="B20" s="14">
         <v>0</v>
@@ -7049,7 +7052,7 @@
     </row>
     <row r="21" spans="1:109" x14ac:dyDescent="0.35">
       <c r="A21" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B21" s="14">
         <v>0</v>
@@ -7378,7 +7381,7 @@
     </row>
     <row r="22" spans="1:109" x14ac:dyDescent="0.35">
       <c r="A22" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B22" s="14">
         <v>0</v>
@@ -7707,7 +7710,7 @@
     </row>
     <row r="23" spans="1:109" x14ac:dyDescent="0.35">
       <c r="A23" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B23" s="14">
         <v>0</v>
@@ -8036,7 +8039,7 @@
     </row>
     <row r="24" spans="1:109" x14ac:dyDescent="0.35">
       <c r="A24" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B24" s="14">
         <v>0</v>
@@ -8365,7 +8368,7 @@
     </row>
     <row r="25" spans="1:109" x14ac:dyDescent="0.35">
       <c r="A25" s="14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B25" s="14">
         <v>0</v>
@@ -8694,7 +8697,7 @@
     </row>
     <row r="26" spans="1:109" x14ac:dyDescent="0.35">
       <c r="A26" s="14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B26" s="14">
         <v>0</v>
@@ -9023,7 +9026,7 @@
     </row>
     <row r="27" spans="1:109" x14ac:dyDescent="0.35">
       <c r="A27" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B27" s="14">
         <v>0</v>
@@ -9352,7 +9355,7 @@
     </row>
     <row r="28" spans="1:109" x14ac:dyDescent="0.35">
       <c r="A28" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B28" s="14">
         <v>0</v>
@@ -9681,7 +9684,7 @@
     </row>
     <row r="29" spans="1:109" x14ac:dyDescent="0.35">
       <c r="A29" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B29" s="14">
         <v>0</v>
@@ -10010,7 +10013,7 @@
     </row>
     <row r="30" spans="1:109" x14ac:dyDescent="0.35">
       <c r="A30" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B30" s="14">
         <v>0</v>
@@ -10339,7 +10342,7 @@
     </row>
     <row r="31" spans="1:109" x14ac:dyDescent="0.35">
       <c r="A31" s="14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B31" s="14">
         <v>0</v>
@@ -10668,7 +10671,7 @@
     </row>
     <row r="32" spans="1:109" x14ac:dyDescent="0.35">
       <c r="A32" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B32" s="14">
         <v>0</v>
@@ -10997,7 +11000,7 @@
     </row>
     <row r="33" spans="1:109" x14ac:dyDescent="0.35">
       <c r="A33" s="14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B33" s="14">
         <v>0</v>
@@ -11326,7 +11329,7 @@
     </row>
     <row r="34" spans="1:109" x14ac:dyDescent="0.35">
       <c r="A34" s="14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B34" s="14">
         <v>0</v>
@@ -11655,7 +11658,7 @@
     </row>
     <row r="35" spans="1:109" x14ac:dyDescent="0.35">
       <c r="A35" s="14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B35" s="14">
         <v>0</v>
@@ -11984,7 +11987,7 @@
     </row>
     <row r="36" spans="1:109" x14ac:dyDescent="0.35">
       <c r="A36" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B36" s="14">
         <v>0</v>
@@ -12313,7 +12316,7 @@
     </row>
     <row r="37" spans="1:109" x14ac:dyDescent="0.35">
       <c r="A37" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B37" s="14">
         <v>0</v>
@@ -12642,7 +12645,7 @@
     </row>
     <row r="38" spans="1:109" x14ac:dyDescent="0.35">
       <c r="A38" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B38" s="14">
         <v>0</v>
@@ -12971,7 +12974,7 @@
     </row>
     <row r="39" spans="1:109" x14ac:dyDescent="0.35">
       <c r="A39" s="14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B39" s="14">
         <v>0</v>
@@ -13300,7 +13303,7 @@
     </row>
     <row r="40" spans="1:109" x14ac:dyDescent="0.35">
       <c r="A40" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B40" s="14">
         <v>0</v>
@@ -13629,7 +13632,7 @@
     </row>
     <row r="41" spans="1:109" x14ac:dyDescent="0.35">
       <c r="A41" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B41" s="14">
         <v>0</v>
@@ -13958,7 +13961,7 @@
     </row>
     <row r="42" spans="1:109" x14ac:dyDescent="0.35">
       <c r="A42" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B42" s="14">
         <v>0</v>
@@ -14287,7 +14290,7 @@
     </row>
     <row r="43" spans="1:109" x14ac:dyDescent="0.35">
       <c r="A43" s="14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B43" s="14">
         <v>1</v>
@@ -14616,7 +14619,7 @@
     </row>
     <row r="44" spans="1:109" x14ac:dyDescent="0.35">
       <c r="A44" s="14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B44" s="14">
         <v>0</v>
@@ -14945,7 +14948,7 @@
     </row>
     <row r="45" spans="1:109" x14ac:dyDescent="0.35">
       <c r="A45" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B45" s="14">
         <v>0</v>
@@ -15274,7 +15277,7 @@
     </row>
     <row r="46" spans="1:109" x14ac:dyDescent="0.35">
       <c r="A46" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B46" s="14">
         <v>0</v>
@@ -15603,7 +15606,7 @@
     </row>
     <row r="47" spans="1:109" x14ac:dyDescent="0.35">
       <c r="A47" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B47" s="14">
         <v>0</v>
@@ -15932,7 +15935,7 @@
     </row>
     <row r="48" spans="1:109" x14ac:dyDescent="0.35">
       <c r="A48" s="14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B48" s="14">
         <v>1</v>
@@ -16261,7 +16264,7 @@
     </row>
     <row r="49" spans="1:109" x14ac:dyDescent="0.35">
       <c r="A49" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B49" s="14">
         <v>0</v>
@@ -16590,7 +16593,7 @@
     </row>
     <row r="50" spans="1:109" x14ac:dyDescent="0.35">
       <c r="A50" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B50" s="14">
         <v>0</v>
@@ -16919,7 +16922,7 @@
     </row>
     <row r="51" spans="1:109" x14ac:dyDescent="0.35">
       <c r="A51" s="14" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="B51" s="14">
         <v>0</v>
@@ -17248,7 +17251,7 @@
     </row>
     <row r="52" spans="1:109" x14ac:dyDescent="0.35">
       <c r="A52" s="14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B52" s="14">
         <v>0</v>
@@ -17577,7 +17580,7 @@
     </row>
     <row r="53" spans="1:109" x14ac:dyDescent="0.35">
       <c r="A53" s="14" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B53" s="14">
         <v>0</v>
@@ -17906,7 +17909,7 @@
     </row>
     <row r="54" spans="1:109" x14ac:dyDescent="0.35">
       <c r="A54" s="14" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B54" s="14">
         <v>0</v>
@@ -18235,7 +18238,7 @@
     </row>
     <row r="55" spans="1:109" x14ac:dyDescent="0.35">
       <c r="A55" s="14" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B55" s="14">
         <v>0</v>
@@ -18564,7 +18567,7 @@
     </row>
     <row r="56" spans="1:109" x14ac:dyDescent="0.35">
       <c r="A56" s="14" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B56" s="14">
         <v>0</v>
@@ -18893,7 +18896,7 @@
     </row>
     <row r="57" spans="1:109" x14ac:dyDescent="0.35">
       <c r="A57" s="14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B57" s="14">
         <v>0</v>
@@ -19222,7 +19225,7 @@
     </row>
     <row r="58" spans="1:109" x14ac:dyDescent="0.35">
       <c r="A58" s="14" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B58" s="14">
         <v>0</v>

</xml_diff>